<commit_message>
Little change for debugging
</commit_message>
<xml_diff>
--- a/cosimulation/static/demo/4_pv_dev/cyder_inputs.xlsx
+++ b/cosimulation/static/demo/4_pv_dev/cyder_inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Jonathan\Desktop\CyDER\cosimulation\static\demo\4_pv_dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRRC\Desktop\CyDER\cosimulation\static\demo\4_pv_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -408,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="170" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="170" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>